<commit_message>
Excel Sheet angepasst und RFCs eingetragen
</commit_message>
<xml_diff>
--- a/DataDictionary/eCH-0160_xIsadg&EAD_v2.0.xlsx
+++ b/DataDictionary/eCH-0160_xIsadg&EAD_v2.0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5970" windowWidth="25260" windowHeight="6030" tabRatio="861" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="5970" windowWidth="10230" windowHeight="1725" tabRatio="861" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="eCH-0160 zu xIsadg v1.6.1" sheetId="13" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <definedName name="_ftnref2" localSheetId="2">xIsadg_DataDictionary!#REF!</definedName>
     <definedName name="_ftnref3" localSheetId="2">xIsadg_DataDictionary!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'eCH-0160 zu xIsadg v1.6.1'!$A$1:$J$42</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'eCH-0160 zu xIsadg v2.0'!$A$1:$I$71</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'eCH-0160 zu xIsadg v2.0'!$A$1:$I$65</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'ISAD(G)'!$A$1:$C$38</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">xIsadg_DataDictionary!$A$1:$H$41</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">xIsadg_DataDictionary!$2:$2</definedName>
@@ -1515,7 +1515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="497">
   <si>
     <t>archivierungsmodusLöschvorschriften</t>
   </si>
@@ -3276,9 +3276,6 @@
     <t>dokument</t>
   </si>
   <si>
-    <t>//arelda:dokument/arelda:titel</t>
-  </si>
-  <si>
     <t>//arelda:dokument/arelda:dokumenttyp</t>
   </si>
   <si>
@@ -3343,9 +3340,6 @@
 //arelda:dokument/arelda:entstehungszeitraum</t>
   </si>
   <si>
-    <t>//arelda:dossier/arelda:umfang</t>
-  </si>
-  <si>
     <t>//arelda:dokument/arelda:autor</t>
   </si>
   <si>
@@ -3394,14 +3388,6 @@
     <t>//arelda:ablieferung/arelda:bemerkung
 //arelda:provenienz/arelda:bemerkung
 //arelda:ordnungssystem/arelda:bemerkung</t>
-  </si>
-  <si>
-    <t>//arelda:paket/arelda:zusatzDaten
-//arelda:ablieferung/arelda:zusatzDaten</t>
-  </si>
-  <si>
-    <t>//arelda:ordnungssystemposition/arelda:zusatzDaten
-//arelda:ordnungssystem/arelda:zusatzDaten</t>
   </si>
   <si>
     <t>//arelda:dossier/arelda:zusatzDaten</t>
@@ -3438,8 +3424,79 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">//arelda:paket/arelda:paketTyp
-//arelda:paket/arelda:schemaVersion
+      <t xml:space="preserve">//arelda:ordnungssystemposition/arelda:/nummer
+//arelda:ordnungssystemposition/arelda:/federfuehrendeOrganisationseinheit
+Zusätzliche Ebene:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>//arelda:ordnungssystemposition/arelda:/zusatzDaten(key/value)</t>
+    </r>
+  </si>
+  <si>
+    <t>//arelda:ordnungssystemposition/arelda:zusatzDaten</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">//arelda:paket/arelda:zusatzDaten
+//arelda:ablieferung/arelda:zusatzDaten
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>//arelda:ordnungssystem/arelda:zusatzDaten</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>//arelda:paket/@xmlns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+//arelda:paket/arelda:paketTyp
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>//arelda:paket/@schemaVersion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
 //arelda:ablieferung/arelda:ablieferungsnummer
 //arelda:ablieferung/arelda:ablieferungstyp
 //arelda:ablieferung/arelda:angebotsnummer
@@ -3486,26 +3543,35 @@
     </r>
   </si>
   <si>
+    <t>GELB</t>
+  </si>
+  <si>
+    <t>noch nicht umgesetzt</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">//arelda:ordnungssystemposition/arelda:/nummer
-//arelda:ordnungssystemposition/arelda:/federfuehrendeOrganisationseinheit
-Zusätzliche Ebene:
+      <t xml:space="preserve">//arelda:dokument/arelda:anwendung
 </t>
     </r>
     <r>
       <rPr>
-        <strike/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">//arelda:datei/arelda:name
+//arelda:datei/arelda:originalName
+</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>//arelda:ordnungssystemposition/arelda:/zusatzDaten(key/value)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">//arelda:dokument/arelda:anwendung
+      <t xml:space="preserve">
 Zusätzliche Ebene:
 </t>
     </r>
@@ -3522,21 +3588,56 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">//arelda:dokument/arelda:titel [GEVER]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>//arelda:datei/arelda:name [FILES]
+//arelda:datei/arelda:originalName [FILES]</t>
+    </r>
+  </si>
+  <si>
+    <t>//arelda:dossier/arelda:umfang [FILES]</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">//arelda:dossier/arelda:federfuehrendeOrganisationseinheit
 //arelda:dossier/arelda:vorgang
-//arelda(v1.1):vorgang/arelda:titel
-//arelda(v1.1):vorgang/arelda:arbeitsanweisung
-//arelda(v1.1):vorgang/arelda:federfuehrung
-//arelda(v1.1):vorgang/arelda:verweis
-//arelda(v1.1):vorgang/arelda:bemerkung
-//arelda(v1.1):vorgang/arelda:order
-//arelda(v1.1):aktivitaet/arelda:vorschreibung
-//arelda(v1.1):aktivitaet/arelda:anweisung
-//arelda(v1.1):aktivitaet/arelda:bearbeiter
-//arelda(v1.1):aktivitaet/arelda:abschlussdatum
-//arelda(v1.1):aktivitaet/arelda:verweis
-//arelda(v1.1):aktivitaet/arelda:bemerkung
-//arelda(v1.1):aktivitaet/arelda:order
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">//arelda:vorgang/arelda:titel [v1.1]
+//arelda:vorgang/arelda:arbeitsanweisung [v1.1]
+//arelda:vorgang/arelda:verweis [v1.1]
+//arelda:vorgang/arelda:aktivitaet/@order [v1.1]
+//arelda:vorgang/arelda:aktivitaet/arelda:vorschreibung [v1.1]
+//arelda:vorgang/arelda:aktivitaet/arelda:akteur [v1.1]
+//arelda:vorgang/arelda:aktivitaet/arelda:abschlussvermerk [v1.1]
+//arelda:vorgang/arelda:aktivitaet/arelda:abschlussdatum [v1.1]
+//arelda:vorgang/arelda:aktivitaet/arelda:verweis [v1.1]
+//arelda:vorgang/arelda:aktivitaet/arelda:bemerkung [v1.1]
 Zusätzliche Ebene:
 </t>
     </r>
@@ -3544,7 +3645,7 @@
       <rPr>
         <strike/>
         <sz val="10"/>
-        <color theme="1"/>
+        <color rgb="FFFFC000"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -3553,12 +3654,22 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color theme="1"/>
+        <color rgb="FFFFC000"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-//arelda(V1.1):vorgang/arelda:zusatzDaten(key/value)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>//arelda(V1.1):vorgang/arelda:zusatzDaten(key/value)
 //arelda(V1.1):aktivitaet/arelda:zusatzDaten(key/value)</t>
     </r>
   </si>
@@ -3567,7 +3678,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="34">
+  <fonts count="37">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3777,6 +3888,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -4746,7 +4876,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="232">
+  <cellXfs count="233">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -5432,6 +5562,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6925,7 +7058,7 @@
   </sheetPr>
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
@@ -6933,7 +7066,7 @@
   <cols>
     <col min="1" max="1" width="57.5703125" style="177" customWidth="1"/>
     <col min="2" max="2" width="66.42578125" style="177" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" style="177" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" style="177" customWidth="1"/>
     <col min="4" max="4" width="55.5703125" style="177" customWidth="1"/>
     <col min="5" max="5" width="2.7109375" style="173" customWidth="1"/>
     <col min="6" max="6" width="19.140625" style="172" customWidth="1"/>
@@ -6943,7 +7076,7 @@
     <col min="10" max="16384" width="58.7109375" style="177"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.75" customHeight="1" thickBot="1">
+    <row r="1" spans="1:9" ht="29.25" customHeight="1" thickBot="1">
       <c r="A1" s="224" t="s">
         <v>429</v>
       </c>
@@ -7015,7 +7148,7 @@
       </c>
       <c r="I4" s="162"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="38.25">
       <c r="A5" s="163" t="s">
         <v>369</v>
       </c>
@@ -7025,8 +7158,8 @@
       <c r="C5" s="163" t="s">
         <v>447</v>
       </c>
-      <c r="D5" s="163" t="s">
-        <v>449</v>
+      <c r="D5" s="164" t="s">
+        <v>494</v>
       </c>
       <c r="E5" s="161"/>
       <c r="F5" s="162"/>
@@ -7055,14 +7188,14 @@
     </row>
     <row r="7" spans="1:9" ht="51.75" customHeight="1">
       <c r="A7" s="164" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B7" s="162"/>
       <c r="C7" s="165" t="s">
+        <v>467</v>
+      </c>
+      <c r="D7" s="165" t="s">
         <v>468</v>
-      </c>
-      <c r="D7" s="165" t="s">
-        <v>469</v>
       </c>
       <c r="E7" s="161"/>
       <c r="F7" s="162"/>
@@ -7140,7 +7273,7 @@
       <c r="A12" s="163"/>
       <c r="B12" s="163"/>
       <c r="C12" s="196" t="s">
-        <v>470</v>
+        <v>495</v>
       </c>
       <c r="D12" s="163"/>
       <c r="I12" s="171" t="s">
@@ -7161,12 +7294,12 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="163" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B14" s="163"/>
       <c r="C14" s="163"/>
       <c r="D14" s="163" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G14" s="169">
         <v>2.1</v>
@@ -7178,7 +7311,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="163" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B15" s="163"/>
       <c r="C15" s="163"/>
@@ -7193,7 +7326,7 @@
     </row>
     <row r="16" spans="1:9" s="172" customFormat="1" ht="63.75">
       <c r="A16" s="198" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B16" s="162"/>
       <c r="C16" s="162"/>
@@ -7209,7 +7342,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="163" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B17" s="163"/>
       <c r="C17" s="163"/>
@@ -7256,10 +7389,10 @@
       <c r="A21" s="163"/>
       <c r="B21" s="163"/>
       <c r="C21" s="163" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D21" s="163" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G21" s="194"/>
       <c r="I21" s="174" t="s">
@@ -7268,11 +7401,11 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="163" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B22" s="163"/>
       <c r="C22" s="163" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D22" s="163"/>
       <c r="G22" s="171"/>
@@ -7282,7 +7415,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="163" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B23" s="163"/>
       <c r="C23" s="163"/>
@@ -7310,7 +7443,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="163" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B25" s="163"/>
       <c r="C25" s="163"/>
@@ -7358,13 +7491,13 @@
     <row r="29" spans="1:9">
       <c r="A29" s="163"/>
       <c r="B29" s="163" t="s">
+        <v>459</v>
+      </c>
+      <c r="C29" s="163" t="s">
         <v>460</v>
       </c>
-      <c r="C29" s="163" t="s">
+      <c r="D29" s="163" t="s">
         <v>461</v>
-      </c>
-      <c r="D29" s="163" t="s">
-        <v>462</v>
       </c>
       <c r="G29" s="194"/>
       <c r="H29" s="162"/>
@@ -7375,13 +7508,13 @@
     <row r="30" spans="1:9">
       <c r="A30" s="163"/>
       <c r="B30" s="163" t="s">
+        <v>453</v>
+      </c>
+      <c r="C30" s="163" t="s">
         <v>454</v>
       </c>
-      <c r="C30" s="163" t="s">
+      <c r="D30" s="163" t="s">
         <v>455</v>
-      </c>
-      <c r="D30" s="163" t="s">
-        <v>456</v>
       </c>
       <c r="G30" s="193"/>
       <c r="H30" s="162"/>
@@ -7392,13 +7525,13 @@
     <row r="31" spans="1:9">
       <c r="A31" s="163"/>
       <c r="B31" s="163" t="s">
+        <v>462</v>
+      </c>
+      <c r="C31" s="163" t="s">
         <v>463</v>
       </c>
-      <c r="C31" s="163" t="s">
+      <c r="D31" s="163" t="s">
         <v>464</v>
-      </c>
-      <c r="D31" s="163" t="s">
-        <v>465</v>
       </c>
       <c r="G31" s="193"/>
       <c r="H31" s="162"/>
@@ -7415,7 +7548,7 @@
         <v>442</v>
       </c>
       <c r="D32" s="163" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G32" s="193"/>
       <c r="H32" s="162"/>
@@ -7426,13 +7559,13 @@
     <row r="33" spans="1:9">
       <c r="A33" s="163"/>
       <c r="B33" s="163" t="s">
+        <v>456</v>
+      </c>
+      <c r="C33" s="163" t="s">
         <v>457</v>
       </c>
-      <c r="C33" s="163" t="s">
+      <c r="D33" s="163" t="s">
         <v>458</v>
-      </c>
-      <c r="D33" s="163" t="s">
-        <v>459</v>
       </c>
       <c r="G33" s="193"/>
       <c r="H33" s="162"/>
@@ -7442,7 +7575,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="163" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B34" s="163" t="s">
         <v>438</v>
@@ -7459,7 +7592,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="163" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B35" s="163" t="s">
         <v>439</v>
@@ -7476,7 +7609,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="163" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B36" s="195" t="s">
         <v>440</v>
@@ -7530,10 +7663,10 @@
       <c r="A40" s="163"/>
       <c r="B40" s="163"/>
       <c r="C40" s="163" t="s">
+        <v>465</v>
+      </c>
+      <c r="D40" s="163" t="s">
         <v>466</v>
-      </c>
-      <c r="D40" s="163" t="s">
-        <v>467</v>
       </c>
       <c r="G40" s="169">
         <v>4.4000000000000004</v>
@@ -7648,14 +7781,14 @@
     </row>
     <row r="50" spans="1:9" ht="38.25">
       <c r="A50" s="164" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B50" s="163"/>
       <c r="C50" s="163" t="s">
+        <v>451</v>
+      </c>
+      <c r="D50" s="163" t="s">
         <v>452</v>
-      </c>
-      <c r="D50" s="163" t="s">
-        <v>453</v>
       </c>
       <c r="G50" s="169">
         <v>6.1</v>
@@ -7751,7 +7884,7 @@
       <c r="A58" s="163"/>
       <c r="B58" s="163"/>
       <c r="C58" s="164" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D58" s="163"/>
       <c r="G58" s="160"/>
@@ -7790,18 +7923,18 @@
       <c r="H61" s="162"/>
       <c r="I61" s="162"/>
     </row>
-    <row r="62" spans="1:9" ht="25.5">
+    <row r="62" spans="1:9" ht="38.25">
       <c r="A62" s="164" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="B62" s="164" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C62" s="164" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D62" s="163" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="G62" s="160"/>
       <c r="H62" s="160" t="s">
@@ -7811,13 +7944,13 @@
     </row>
     <row r="63" spans="1:9" ht="275.25" customHeight="1">
       <c r="A63" s="164" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B63" s="164" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="C63" s="176" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="D63" s="176" t="s">
         <v>493</v>
@@ -7840,48 +7973,56 @@
       </c>
       <c r="I65" s="169"/>
     </row>
+    <row r="67" spans="5:9">
+      <c r="E67" s="189"/>
+      <c r="F67" s="178" t="s">
+        <v>419</v>
+      </c>
+      <c r="G67" s="172" t="s">
+        <v>420</v>
+      </c>
+    </row>
     <row r="68" spans="5:9">
-      <c r="E68" s="189"/>
-      <c r="F68" s="178" t="s">
-        <v>419</v>
+      <c r="E68" s="190"/>
+      <c r="F68" s="179" t="s">
+        <v>421</v>
       </c>
       <c r="G68" s="172" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="69" spans="5:9">
-      <c r="E69" s="190"/>
-      <c r="F69" s="179" t="s">
-        <v>421</v>
+      <c r="E69" s="191"/>
+      <c r="F69" s="180" t="s">
+        <v>423</v>
       </c>
       <c r="G69" s="172" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="70" spans="5:9">
-      <c r="E70" s="191"/>
-      <c r="F70" s="180" t="s">
-        <v>423</v>
-      </c>
-      <c r="G70" s="172" t="s">
-        <v>424</v>
+      <c r="E70" s="192"/>
+      <c r="F70" s="181" t="s">
+        <v>425</v>
+      </c>
+      <c r="G70" s="182" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="71" spans="5:9">
-      <c r="E71" s="192"/>
-      <c r="F71" s="181" t="s">
-        <v>425</v>
-      </c>
-      <c r="G71" s="182" t="s">
-        <v>426</v>
+      <c r="F71" s="197" t="s">
+        <v>435</v>
+      </c>
+      <c r="G71" s="172" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="72" spans="5:9">
-      <c r="F72" s="197" t="s">
-        <v>435</v>
+      <c r="F72" s="232" t="s">
+        <v>491</v>
       </c>
       <c r="G72" s="172" t="s">
-        <v>436</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -7909,8 +8050,8 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="43" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="46" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Excel Druckbereich richtig setzten
</commit_message>
<xml_diff>
--- a/DataDictionary/eCH-0160_xIsadg&EAD_v2.0.xlsx
+++ b/DataDictionary/eCH-0160_xIsadg&EAD_v2.0.xlsx
@@ -5134,6 +5134,24 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -5235,24 +5253,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5729,18 +5729,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A1" s="180" t="s">
+      <c r="A1" s="186" t="s">
         <v>336</v>
       </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
+      <c r="E1" s="186"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="186"/>
+      <c r="H1" s="186"/>
+      <c r="I1" s="186"/>
+      <c r="J1" s="186"/>
     </row>
     <row r="2" spans="1:10" ht="13.5" thickBot="1">
       <c r="A2" s="3" t="s">
@@ -5773,11 +5773,11 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="13.5" thickBot="1">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="198" t="s">
         <v>167</v>
       </c>
-      <c r="B3" s="193"/>
-      <c r="C3" s="194"/>
+      <c r="B3" s="199"/>
+      <c r="C3" s="200"/>
       <c r="D3" s="36" t="s">
         <v>211</v>
       </c>
@@ -5859,14 +5859,14 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="13.5" thickBot="1">
-      <c r="A7" s="199" t="s">
+      <c r="A7" s="205" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="200"/>
-      <c r="C7" s="200"/>
-      <c r="D7" s="200"/>
-      <c r="E7" s="200"/>
-      <c r="F7" s="201"/>
+      <c r="B7" s="206"/>
+      <c r="C7" s="206"/>
+      <c r="D7" s="206"/>
+      <c r="E7" s="206"/>
+      <c r="F7" s="207"/>
       <c r="G7" s="67"/>
       <c r="H7" s="2" t="s">
         <v>53</v>
@@ -5935,11 +5935,11 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="13.5" thickBot="1">
-      <c r="A11" s="196" t="s">
+      <c r="A11" s="202" t="s">
         <v>170</v>
       </c>
-      <c r="B11" s="197"/>
-      <c r="C11" s="198"/>
+      <c r="B11" s="203"/>
+      <c r="C11" s="204"/>
       <c r="D11" s="24" t="s">
         <v>18</v>
       </c>
@@ -6207,7 +6207,7 @@
       <c r="F24" s="63"/>
       <c r="G24" s="69"/>
       <c r="H24" s="42"/>
-      <c r="J24" s="181" t="s">
+      <c r="J24" s="187" t="s">
         <v>206</v>
       </c>
     </row>
@@ -6226,7 +6226,7 @@
       <c r="F25" s="72"/>
       <c r="G25" s="19"/>
       <c r="H25" s="42"/>
-      <c r="J25" s="182"/>
+      <c r="J25" s="188"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="25" t="s">
@@ -6243,7 +6243,7 @@
       <c r="F26" s="18"/>
       <c r="G26" s="69"/>
       <c r="H26" s="42"/>
-      <c r="J26" s="182"/>
+      <c r="J26" s="188"/>
     </row>
     <row r="27" spans="1:10" ht="13.5" thickBot="1">
       <c r="A27" s="76"/>
@@ -6258,7 +6258,7 @@
       <c r="F27" s="72"/>
       <c r="G27" s="19"/>
       <c r="H27" s="42"/>
-      <c r="J27" s="182"/>
+      <c r="J27" s="188"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" customHeight="1">
       <c r="A28" s="52"/>
@@ -6274,13 +6274,13 @@
         <v>19</v>
       </c>
       <c r="G28" s="85"/>
-      <c r="H28" s="184" t="s">
+      <c r="H28" s="190" t="s">
         <v>64</v>
       </c>
-      <c r="I28" s="187" t="s">
+      <c r="I28" s="193" t="s">
         <v>185</v>
       </c>
-      <c r="J28" s="182"/>
+      <c r="J28" s="188"/>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="52"/>
@@ -6296,9 +6296,9 @@
         <v>9</v>
       </c>
       <c r="G29" s="19"/>
-      <c r="H29" s="185"/>
-      <c r="I29" s="188"/>
-      <c r="J29" s="182"/>
+      <c r="H29" s="191"/>
+      <c r="I29" s="194"/>
+      <c r="J29" s="188"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="52"/>
@@ -6314,9 +6314,9 @@
         <v>14</v>
       </c>
       <c r="G30" s="19"/>
-      <c r="H30" s="185"/>
-      <c r="I30" s="188"/>
-      <c r="J30" s="182"/>
+      <c r="H30" s="191"/>
+      <c r="I30" s="194"/>
+      <c r="J30" s="188"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" customHeight="1">
       <c r="A31" s="52"/>
@@ -6332,9 +6332,9 @@
         <v>34</v>
       </c>
       <c r="G31" s="83"/>
-      <c r="H31" s="185"/>
-      <c r="I31" s="188"/>
-      <c r="J31" s="182"/>
+      <c r="H31" s="191"/>
+      <c r="I31" s="194"/>
+      <c r="J31" s="188"/>
     </row>
     <row r="32" spans="1:10" ht="13.5" thickBot="1">
       <c r="A32" s="52"/>
@@ -6350,9 +6350,9 @@
         <v>13</v>
       </c>
       <c r="G32" s="11"/>
-      <c r="H32" s="186"/>
-      <c r="I32" s="189"/>
-      <c r="J32" s="183"/>
+      <c r="H32" s="192"/>
+      <c r="I32" s="195"/>
+      <c r="J32" s="189"/>
     </row>
     <row r="33" spans="1:10" ht="13.5" thickBot="1">
       <c r="A33" s="53"/>
@@ -6485,10 +6485,10 @@
       <c r="J39" s="119"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="195" t="s">
+      <c r="A40" s="201" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="195"/>
+      <c r="B40" s="201"/>
       <c r="C40" s="46"/>
       <c r="D40" s="44"/>
       <c r="E40" s="44"/>
@@ -6498,10 +6498,10 @@
       <c r="J40" s="119"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="195" t="s">
+      <c r="A41" s="201" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="195"/>
+      <c r="B41" s="201"/>
       <c r="C41" s="47"/>
       <c r="D41" s="44"/>
       <c r="E41" s="44"/>
@@ -6511,10 +6511,10 @@
       <c r="J41" s="119"/>
     </row>
     <row r="42" spans="1:10" ht="26.25" customHeight="1">
-      <c r="A42" s="190" t="s">
+      <c r="A42" s="196" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="191"/>
+      <c r="B42" s="197"/>
       <c r="C42" s="48"/>
       <c r="D42" s="44"/>
       <c r="E42" s="44"/>
@@ -6789,8 +6789,8 @@
   </sheetPr>
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F53" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L68" sqref="A1:L68"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="58.7109375" defaultRowHeight="12.75"/>
@@ -6811,28 +6811,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A1" s="202" t="s">
+      <c r="A1" s="208" t="s">
         <v>335</v>
       </c>
-      <c r="B1" s="202"/>
-      <c r="C1" s="202"/>
-      <c r="D1" s="202"/>
-      <c r="E1" s="202"/>
-      <c r="F1" s="202"/>
-      <c r="G1" s="202"/>
-      <c r="H1" s="202"/>
-      <c r="I1" s="202"/>
-      <c r="J1" s="202"/>
-      <c r="K1" s="202"/>
-      <c r="L1" s="202"/>
+      <c r="B1" s="208"/>
+      <c r="C1" s="208"/>
+      <c r="D1" s="208"/>
+      <c r="E1" s="208"/>
+      <c r="F1" s="208"/>
+      <c r="G1" s="208"/>
+      <c r="H1" s="208"/>
+      <c r="I1" s="208"/>
+      <c r="J1" s="208"/>
+      <c r="K1" s="208"/>
+      <c r="L1" s="208"/>
     </row>
     <row r="2" spans="1:13" s="147" customFormat="1">
-      <c r="A2" s="203" t="s">
+      <c r="A2" s="209" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="204"/>
-      <c r="C2" s="204"/>
-      <c r="D2" s="204"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
       <c r="E2" s="163" t="s">
         <v>211</v>
       </c>
@@ -6842,13 +6842,13 @@
       <c r="G2" s="164" t="s">
         <v>169</v>
       </c>
-      <c r="H2" s="205" t="s">
+      <c r="H2" s="211" t="s">
         <v>333</v>
       </c>
-      <c r="I2" s="206"/>
-      <c r="J2" s="206"/>
-      <c r="K2" s="206"/>
-      <c r="L2" s="207"/>
+      <c r="I2" s="212"/>
+      <c r="J2" s="212"/>
+      <c r="K2" s="212"/>
+      <c r="L2" s="213"/>
     </row>
     <row r="3" spans="1:13" s="147" customFormat="1" ht="13.5" thickBot="1">
       <c r="A3" s="159" t="s">
@@ -6872,21 +6872,21 @@
       <c r="G3" s="148" t="s">
         <v>349</v>
       </c>
-      <c r="H3" s="208" t="s">
+      <c r="H3" s="214" t="s">
         <v>289</v>
       </c>
-      <c r="I3" s="209"/>
-      <c r="J3" s="209"/>
-      <c r="K3" s="209"/>
-      <c r="L3" s="210"/>
+      <c r="I3" s="215"/>
+      <c r="J3" s="215"/>
+      <c r="K3" s="215"/>
+      <c r="L3" s="216"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="144"/>
       <c r="B4" s="144"/>
       <c r="C4" s="165"/>
       <c r="D4" s="165"/>
-      <c r="E4" s="215"/>
-      <c r="F4" s="216"/>
+      <c r="E4" s="181"/>
+      <c r="F4" s="182"/>
       <c r="G4" s="165"/>
       <c r="H4" s="149">
         <v>1</v>
@@ -6905,10 +6905,10 @@
       </c>
       <c r="C5" s="165"/>
       <c r="D5" s="165"/>
-      <c r="E5" s="216" t="s">
+      <c r="E5" s="182" t="s">
         <v>286</v>
       </c>
-      <c r="F5" s="216" t="s">
+      <c r="F5" s="182" t="s">
         <v>286</v>
       </c>
       <c r="G5" s="165" t="s">
@@ -6931,10 +6931,10 @@
       </c>
       <c r="C6" s="165"/>
       <c r="D6" s="165"/>
-      <c r="E6" s="216" t="s">
+      <c r="E6" s="182" t="s">
         <v>350</v>
       </c>
-      <c r="F6" s="216" t="s">
+      <c r="F6" s="182" t="s">
         <v>351</v>
       </c>
       <c r="G6" s="165" t="s">
@@ -6955,9 +6955,9 @@
       <c r="B7" s="144"/>
       <c r="C7" s="165"/>
       <c r="D7" s="165"/>
-      <c r="E7" s="217"/>
-      <c r="F7" s="217"/>
-      <c r="G7" s="219"/>
+      <c r="E7" s="183"/>
+      <c r="F7" s="183"/>
+      <c r="G7" s="185"/>
       <c r="H7" s="150"/>
       <c r="I7" s="169"/>
       <c r="J7" s="143">
@@ -6974,12 +6974,12 @@
         <v>352</v>
       </c>
       <c r="C8" s="165"/>
-      <c r="D8" s="218"/>
-      <c r="E8" s="217"/>
-      <c r="F8" s="217" t="s">
+      <c r="D8" s="184"/>
+      <c r="E8" s="183"/>
+      <c r="F8" s="183" t="s">
         <v>353</v>
       </c>
-      <c r="G8" s="219" t="s">
+      <c r="G8" s="185" t="s">
         <v>354</v>
       </c>
       <c r="H8" s="150"/>
@@ -6997,11 +6997,11 @@
         <v>285</v>
       </c>
       <c r="C9" s="165"/>
-      <c r="D9" s="218"/>
-      <c r="E9" s="216" t="s">
+      <c r="D9" s="184"/>
+      <c r="E9" s="182" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="216" t="s">
+      <c r="F9" s="182" t="s">
         <v>286</v>
       </c>
       <c r="G9" s="165" t="s">
@@ -7021,9 +7021,9 @@
       <c r="A10" s="165"/>
       <c r="B10" s="165"/>
       <c r="C10" s="165"/>
-      <c r="D10" s="218"/>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="182"/>
+      <c r="F10" s="182"/>
       <c r="G10" s="165"/>
       <c r="H10" s="150"/>
       <c r="I10" s="169"/>
@@ -7039,9 +7039,9 @@
       <c r="A11" s="165"/>
       <c r="B11" s="165"/>
       <c r="C11" s="165"/>
-      <c r="D11" s="218"/>
-      <c r="E11" s="216"/>
-      <c r="F11" s="216"/>
+      <c r="D11" s="184"/>
+      <c r="E11" s="182"/>
+      <c r="F11" s="182"/>
       <c r="G11" s="165"/>
       <c r="H11" s="150"/>
       <c r="I11" s="169"/>
@@ -7056,9 +7056,9 @@
       <c r="A12" s="165"/>
       <c r="B12" s="165"/>
       <c r="C12" s="165"/>
-      <c r="D12" s="218"/>
-      <c r="E12" s="216"/>
-      <c r="F12" s="216"/>
+      <c r="D12" s="184"/>
+      <c r="E12" s="182"/>
+      <c r="F12" s="182"/>
       <c r="G12" s="165"/>
       <c r="H12" s="150"/>
       <c r="I12" s="169"/>
@@ -7073,9 +7073,9 @@
       <c r="A13" s="165"/>
       <c r="B13" s="165"/>
       <c r="C13" s="165"/>
-      <c r="D13" s="218"/>
-      <c r="E13" s="216"/>
-      <c r="F13" s="217" t="s">
+      <c r="D13" s="184"/>
+      <c r="E13" s="182"/>
+      <c r="F13" s="183" t="s">
         <v>405</v>
       </c>
       <c r="G13" s="165"/>
@@ -7088,9 +7088,9 @@
       <c r="A14" s="165"/>
       <c r="B14" s="165"/>
       <c r="C14" s="165"/>
-      <c r="D14" s="218"/>
-      <c r="E14" s="216"/>
-      <c r="F14" s="216"/>
+      <c r="D14" s="184"/>
+      <c r="E14" s="182"/>
+      <c r="F14" s="182"/>
       <c r="G14" s="165"/>
       <c r="H14" s="153">
         <v>2</v>
@@ -7105,11 +7105,11 @@
       <c r="C15" s="165" t="s">
         <v>355</v>
       </c>
-      <c r="D15" s="218"/>
-      <c r="E15" s="216" t="s">
+      <c r="D15" s="184"/>
+      <c r="E15" s="182" t="s">
         <v>406</v>
       </c>
-      <c r="F15" s="216" t="s">
+      <c r="F15" s="182" t="s">
         <v>409</v>
       </c>
       <c r="G15" s="165" t="s">
@@ -7129,9 +7129,9 @@
       <c r="C16" s="165" t="s">
         <v>411</v>
       </c>
-      <c r="D16" s="218"/>
-      <c r="E16" s="216"/>
-      <c r="F16" s="216"/>
+      <c r="D16" s="184"/>
+      <c r="E16" s="182"/>
+      <c r="F16" s="182"/>
       <c r="G16" s="165"/>
       <c r="J16" s="143">
         <v>2.2000000000000002</v>
@@ -7147,10 +7147,10 @@
       <c r="C17" s="165" t="s">
         <v>403</v>
       </c>
-      <c r="D17" s="218"/>
-      <c r="E17" s="217"/>
-      <c r="F17" s="217"/>
-      <c r="G17" s="219"/>
+      <c r="D17" s="184"/>
+      <c r="E17" s="183"/>
+      <c r="F17" s="183"/>
+      <c r="G17" s="185"/>
       <c r="H17" s="152"/>
       <c r="I17" s="171"/>
       <c r="J17" s="143">
@@ -7169,9 +7169,9 @@
         <v>415</v>
       </c>
       <c r="C18" s="165"/>
-      <c r="D18" s="218"/>
-      <c r="E18" s="216"/>
-      <c r="F18" s="216"/>
+      <c r="D18" s="184"/>
+      <c r="E18" s="182"/>
+      <c r="F18" s="182"/>
       <c r="G18" s="165"/>
       <c r="J18" s="143">
         <v>2.4</v>
@@ -7185,18 +7185,18 @@
       <c r="A19" s="165"/>
       <c r="B19" s="165"/>
       <c r="C19" s="165"/>
-      <c r="D19" s="218"/>
-      <c r="E19" s="216"/>
-      <c r="F19" s="216"/>
+      <c r="D19" s="184"/>
+      <c r="E19" s="182"/>
+      <c r="F19" s="182"/>
       <c r="G19" s="165"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="165"/>
       <c r="B20" s="165"/>
       <c r="C20" s="165"/>
-      <c r="D20" s="218"/>
-      <c r="E20" s="216"/>
-      <c r="F20" s="216"/>
+      <c r="D20" s="184"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
       <c r="G20" s="165"/>
       <c r="H20" s="153">
         <v>3</v>
@@ -7209,9 +7209,9 @@
       <c r="A21" s="144"/>
       <c r="B21" s="144"/>
       <c r="C21" s="165"/>
-      <c r="D21" s="218"/>
-      <c r="E21" s="216"/>
-      <c r="F21" s="216"/>
+      <c r="D21" s="184"/>
+      <c r="E21" s="182"/>
+      <c r="F21" s="182"/>
       <c r="G21" s="165"/>
       <c r="J21" s="167">
         <v>3.1</v>
@@ -7224,9 +7224,9 @@
       <c r="A22" s="144"/>
       <c r="B22" s="144"/>
       <c r="C22" s="165"/>
-      <c r="D22" s="218"/>
-      <c r="E22" s="216"/>
-      <c r="F22" s="216" t="s">
+      <c r="D22" s="184"/>
+      <c r="E22" s="182"/>
+      <c r="F22" s="182" t="s">
         <v>357</v>
       </c>
       <c r="G22" s="165" t="s">
@@ -7243,9 +7243,9 @@
         <v>359</v>
       </c>
       <c r="C23" s="165"/>
-      <c r="D23" s="218"/>
-      <c r="E23" s="216"/>
-      <c r="F23" s="216" t="s">
+      <c r="D23" s="184"/>
+      <c r="E23" s="182"/>
+      <c r="F23" s="182" t="s">
         <v>360</v>
       </c>
       <c r="G23" s="165"/>
@@ -7261,9 +7261,9 @@
         <v>361</v>
       </c>
       <c r="C24" s="165"/>
-      <c r="D24" s="218"/>
-      <c r="E24" s="216"/>
-      <c r="F24" s="216"/>
+      <c r="D24" s="184"/>
+      <c r="E24" s="182"/>
+      <c r="F24" s="182"/>
       <c r="G24" s="165"/>
       <c r="J24" s="167">
         <v>3.2</v>
@@ -7277,9 +7277,9 @@
       <c r="A25" s="144"/>
       <c r="B25" s="144"/>
       <c r="C25" s="165"/>
-      <c r="D25" s="218"/>
-      <c r="E25" s="216"/>
-      <c r="F25" s="216"/>
+      <c r="D25" s="184"/>
+      <c r="E25" s="182"/>
+      <c r="F25" s="182"/>
       <c r="G25" s="165"/>
       <c r="J25" s="167">
         <v>3.3</v>
@@ -7293,11 +7293,11 @@
       <c r="A26" s="144"/>
       <c r="B26" s="144"/>
       <c r="C26" s="165"/>
-      <c r="D26" s="218" t="s">
+      <c r="D26" s="184" t="s">
         <v>412</v>
       </c>
-      <c r="E26" s="216"/>
-      <c r="F26" s="216"/>
+      <c r="E26" s="182"/>
+      <c r="F26" s="182"/>
       <c r="G26" s="165" t="s">
         <v>414</v>
       </c>
@@ -7313,9 +7313,9 @@
       <c r="A27" s="144"/>
       <c r="B27" s="144"/>
       <c r="C27" s="165"/>
-      <c r="D27" s="218"/>
-      <c r="E27" s="216"/>
-      <c r="F27" s="216"/>
+      <c r="D27" s="184"/>
+      <c r="E27" s="182"/>
+      <c r="F27" s="182"/>
       <c r="G27" s="165"/>
       <c r="L27" s="169"/>
     </row>
@@ -7323,9 +7323,9 @@
       <c r="A28" s="144"/>
       <c r="B28" s="144"/>
       <c r="C28" s="165"/>
-      <c r="D28" s="218"/>
-      <c r="E28" s="216"/>
-      <c r="F28" s="216"/>
+      <c r="D28" s="184"/>
+      <c r="E28" s="182"/>
+      <c r="F28" s="182"/>
       <c r="G28" s="165"/>
       <c r="H28" s="153">
         <v>4</v>
@@ -7338,9 +7338,9 @@
       <c r="A29" s="144"/>
       <c r="B29" s="144"/>
       <c r="C29" s="165"/>
-      <c r="D29" s="218"/>
-      <c r="E29" s="216"/>
-      <c r="F29" s="216"/>
+      <c r="D29" s="184"/>
+      <c r="E29" s="182"/>
+      <c r="F29" s="182"/>
       <c r="G29" s="165"/>
       <c r="J29" s="143">
         <v>4.0999999999999996</v>
@@ -7354,11 +7354,11 @@
       <c r="A30" s="144"/>
       <c r="B30" s="144"/>
       <c r="C30" s="165"/>
-      <c r="D30" s="218"/>
-      <c r="E30" s="216" t="s">
+      <c r="D30" s="184"/>
+      <c r="E30" s="182" t="s">
         <v>362</v>
       </c>
-      <c r="F30" s="216" t="s">
+      <c r="F30" s="182" t="s">
         <v>363</v>
       </c>
       <c r="G30" s="165" t="s">
@@ -7374,11 +7374,11 @@
       <c r="A31" s="144"/>
       <c r="B31" s="144"/>
       <c r="C31" s="165"/>
-      <c r="D31" s="218"/>
-      <c r="E31" s="216" t="s">
+      <c r="D31" s="184"/>
+      <c r="E31" s="182" t="s">
         <v>365</v>
       </c>
-      <c r="F31" s="216" t="s">
+      <c r="F31" s="182" t="s">
         <v>366</v>
       </c>
       <c r="G31" s="165" t="s">
@@ -7395,11 +7395,11 @@
       <c r="A32" s="144"/>
       <c r="B32" s="144"/>
       <c r="C32" s="165"/>
-      <c r="D32" s="218"/>
-      <c r="E32" s="216" t="s">
+      <c r="D32" s="184"/>
+      <c r="E32" s="182" t="s">
         <v>368</v>
       </c>
-      <c r="F32" s="216" t="s">
+      <c r="F32" s="182" t="s">
         <v>369</v>
       </c>
       <c r="G32" s="165" t="s">
@@ -7416,11 +7416,11 @@
       <c r="A33" s="144"/>
       <c r="B33" s="144"/>
       <c r="C33" s="165"/>
-      <c r="D33" s="218"/>
-      <c r="E33" s="216" t="s">
+      <c r="D33" s="184"/>
+      <c r="E33" s="182" t="s">
         <v>371</v>
       </c>
-      <c r="F33" s="216" t="s">
+      <c r="F33" s="182" t="s">
         <v>372</v>
       </c>
       <c r="G33" s="165" t="s">
@@ -7437,11 +7437,11 @@
       <c r="A34" s="144"/>
       <c r="B34" s="144"/>
       <c r="C34" s="165"/>
-      <c r="D34" s="218"/>
-      <c r="E34" s="216" t="s">
+      <c r="D34" s="184"/>
+      <c r="E34" s="182" t="s">
         <v>374</v>
       </c>
-      <c r="F34" s="216" t="s">
+      <c r="F34" s="182" t="s">
         <v>375</v>
       </c>
       <c r="G34" s="165" t="s">
@@ -7460,11 +7460,11 @@
         <v>377</v>
       </c>
       <c r="C35" s="165"/>
-      <c r="D35" s="218"/>
-      <c r="E35" s="216" t="s">
+      <c r="D35" s="184"/>
+      <c r="E35" s="182" t="s">
         <v>378</v>
       </c>
-      <c r="F35" s="216" t="s">
+      <c r="F35" s="182" t="s">
         <v>379</v>
       </c>
       <c r="G35" s="165"/>
@@ -7480,11 +7480,11 @@
         <v>380</v>
       </c>
       <c r="C36" s="165"/>
-      <c r="D36" s="218"/>
-      <c r="E36" s="216" t="s">
+      <c r="D36" s="184"/>
+      <c r="E36" s="182" t="s">
         <v>381</v>
       </c>
-      <c r="F36" s="216" t="s">
+      <c r="F36" s="182" t="s">
         <v>382</v>
       </c>
       <c r="G36" s="165"/>
@@ -7501,11 +7501,11 @@
         <v>383</v>
       </c>
       <c r="C37" s="165"/>
-      <c r="D37" s="218"/>
-      <c r="E37" s="216" t="s">
+      <c r="D37" s="184"/>
+      <c r="E37" s="182" t="s">
         <v>384</v>
       </c>
-      <c r="F37" s="216" t="s">
+      <c r="F37" s="182" t="s">
         <v>385</v>
       </c>
       <c r="G37" s="165"/>
@@ -7519,9 +7519,9 @@
       <c r="A38" s="144"/>
       <c r="B38" s="144"/>
       <c r="C38" s="165"/>
-      <c r="D38" s="218"/>
-      <c r="E38" s="216"/>
-      <c r="F38" s="216"/>
+      <c r="D38" s="184"/>
+      <c r="E38" s="182"/>
+      <c r="F38" s="182"/>
       <c r="G38" s="165"/>
       <c r="J38" s="175"/>
       <c r="K38" s="169"/>
@@ -7531,9 +7531,9 @@
       <c r="A39" s="144"/>
       <c r="B39" s="144"/>
       <c r="C39" s="165"/>
-      <c r="D39" s="218"/>
-      <c r="E39" s="216"/>
-      <c r="F39" s="216"/>
+      <c r="D39" s="184"/>
+      <c r="E39" s="182"/>
+      <c r="F39" s="182"/>
       <c r="G39" s="165"/>
       <c r="J39" s="143">
         <v>4.2</v>
@@ -7547,9 +7547,9 @@
       <c r="A40" s="144"/>
       <c r="B40" s="144"/>
       <c r="C40" s="165"/>
-      <c r="D40" s="218"/>
-      <c r="E40" s="216"/>
-      <c r="F40" s="216"/>
+      <c r="D40" s="184"/>
+      <c r="E40" s="182"/>
+      <c r="F40" s="182"/>
       <c r="G40" s="165"/>
       <c r="J40" s="143">
         <v>4.3</v>
@@ -7563,9 +7563,9 @@
       <c r="A41" s="144"/>
       <c r="B41" s="144"/>
       <c r="C41" s="165"/>
-      <c r="D41" s="218"/>
-      <c r="E41" s="216"/>
-      <c r="F41" s="216" t="s">
+      <c r="D41" s="184"/>
+      <c r="E41" s="182"/>
+      <c r="F41" s="182" t="s">
         <v>386</v>
       </c>
       <c r="G41" s="165" t="s">
@@ -7583,9 +7583,9 @@
       <c r="A42" s="144"/>
       <c r="B42" s="144"/>
       <c r="C42" s="165"/>
-      <c r="D42" s="218"/>
-      <c r="E42" s="216"/>
-      <c r="F42" s="216"/>
+      <c r="D42" s="184"/>
+      <c r="E42" s="182"/>
+      <c r="F42" s="182"/>
       <c r="G42" s="165"/>
       <c r="J42" s="143">
         <v>4.5</v>
@@ -7599,9 +7599,9 @@
       <c r="A43" s="144"/>
       <c r="B43" s="144"/>
       <c r="C43" s="165"/>
-      <c r="D43" s="218"/>
-      <c r="E43" s="216"/>
-      <c r="F43" s="216"/>
+      <c r="D43" s="184"/>
+      <c r="E43" s="182"/>
+      <c r="F43" s="182"/>
       <c r="G43" s="165"/>
       <c r="K43" s="169"/>
       <c r="L43" s="169"/>
@@ -7610,9 +7610,9 @@
       <c r="A44" s="144"/>
       <c r="B44" s="144"/>
       <c r="C44" s="165"/>
-      <c r="D44" s="218"/>
-      <c r="E44" s="216"/>
-      <c r="F44" s="216"/>
+      <c r="D44" s="184"/>
+      <c r="E44" s="182"/>
+      <c r="F44" s="182"/>
       <c r="G44" s="165"/>
       <c r="H44" s="153">
         <v>5</v>
@@ -7625,9 +7625,9 @@
       <c r="A45" s="144"/>
       <c r="B45" s="144"/>
       <c r="C45" s="165"/>
-      <c r="D45" s="218"/>
-      <c r="E45" s="216"/>
-      <c r="F45" s="216"/>
+      <c r="D45" s="184"/>
+      <c r="E45" s="182"/>
+      <c r="F45" s="182"/>
       <c r="G45" s="165"/>
       <c r="J45" s="167">
         <v>5.0999999999999996</v>
@@ -7640,9 +7640,9 @@
       <c r="A46" s="144"/>
       <c r="B46" s="144"/>
       <c r="C46" s="165"/>
-      <c r="D46" s="218"/>
-      <c r="E46" s="216"/>
-      <c r="F46" s="216"/>
+      <c r="D46" s="184"/>
+      <c r="E46" s="182"/>
+      <c r="F46" s="182"/>
       <c r="G46" s="165"/>
       <c r="J46" s="167">
         <v>5.2</v>
@@ -7655,9 +7655,9 @@
       <c r="A47" s="144"/>
       <c r="B47" s="144"/>
       <c r="C47" s="165"/>
-      <c r="D47" s="218"/>
-      <c r="E47" s="216"/>
-      <c r="F47" s="216"/>
+      <c r="D47" s="184"/>
+      <c r="E47" s="182"/>
+      <c r="F47" s="182"/>
       <c r="G47" s="165"/>
       <c r="J47" s="167">
         <v>5.3</v>
@@ -7670,9 +7670,9 @@
       <c r="A48" s="144"/>
       <c r="B48" s="144"/>
       <c r="C48" s="165"/>
-      <c r="D48" s="218"/>
-      <c r="E48" s="216"/>
-      <c r="F48" s="216"/>
+      <c r="D48" s="184"/>
+      <c r="E48" s="182"/>
+      <c r="F48" s="182"/>
       <c r="G48" s="165"/>
       <c r="J48" s="167">
         <v>5.4</v>
@@ -7685,9 +7685,9 @@
       <c r="A49" s="144"/>
       <c r="B49" s="144"/>
       <c r="C49" s="165"/>
-      <c r="D49" s="218"/>
-      <c r="E49" s="216"/>
-      <c r="F49" s="216"/>
+      <c r="D49" s="184"/>
+      <c r="E49" s="182"/>
+      <c r="F49" s="182"/>
       <c r="G49" s="165"/>
       <c r="K49" s="169"/>
       <c r="L49" s="169"/>
@@ -7696,9 +7696,9 @@
       <c r="A50" s="144"/>
       <c r="B50" s="144"/>
       <c r="C50" s="165"/>
-      <c r="D50" s="218"/>
-      <c r="E50" s="216"/>
-      <c r="F50" s="216"/>
+      <c r="D50" s="184"/>
+      <c r="E50" s="182"/>
+      <c r="F50" s="182"/>
       <c r="G50" s="165"/>
       <c r="H50" s="153">
         <v>6</v>
@@ -7717,11 +7717,11 @@
       <c r="C51" s="165" t="s">
         <v>389</v>
       </c>
-      <c r="D51" s="218" t="s">
+      <c r="D51" s="184" t="s">
         <v>390</v>
       </c>
-      <c r="E51" s="216"/>
-      <c r="F51" s="216" t="s">
+      <c r="E51" s="182"/>
+      <c r="F51" s="182" t="s">
         <v>391</v>
       </c>
       <c r="G51" s="165" t="s">
@@ -7739,9 +7739,9 @@
       <c r="A52" s="144"/>
       <c r="B52" s="144"/>
       <c r="C52" s="165"/>
-      <c r="D52" s="218"/>
-      <c r="E52" s="216"/>
-      <c r="F52" s="216"/>
+      <c r="D52" s="184"/>
+      <c r="E52" s="182"/>
+      <c r="F52" s="182"/>
       <c r="G52" s="165"/>
       <c r="K52" s="169"/>
       <c r="L52" s="169"/>
@@ -7750,9 +7750,9 @@
       <c r="A53" s="144"/>
       <c r="B53" s="144"/>
       <c r="C53" s="165"/>
-      <c r="D53" s="218"/>
-      <c r="E53" s="216"/>
-      <c r="F53" s="216"/>
+      <c r="D53" s="184"/>
+      <c r="E53" s="182"/>
+      <c r="F53" s="182"/>
       <c r="G53" s="165"/>
       <c r="H53" s="153">
         <v>7</v>
@@ -7767,9 +7767,9 @@
       <c r="A54" s="144"/>
       <c r="B54" s="144"/>
       <c r="C54" s="165"/>
-      <c r="D54" s="218"/>
-      <c r="E54" s="216"/>
-      <c r="F54" s="216"/>
+      <c r="D54" s="184"/>
+      <c r="E54" s="182"/>
+      <c r="F54" s="182"/>
       <c r="G54" s="165"/>
       <c r="J54" s="143">
         <v>7.1</v>
@@ -7783,9 +7783,9 @@
       <c r="A55" s="144"/>
       <c r="B55" s="144"/>
       <c r="C55" s="165"/>
-      <c r="D55" s="218"/>
-      <c r="E55" s="216"/>
-      <c r="F55" s="216"/>
+      <c r="D55" s="184"/>
+      <c r="E55" s="182"/>
+      <c r="F55" s="182"/>
       <c r="G55" s="165"/>
       <c r="J55" s="143">
         <v>7.2</v>
@@ -7799,9 +7799,9 @@
       <c r="A56" s="144"/>
       <c r="B56" s="144"/>
       <c r="C56" s="165"/>
-      <c r="D56" s="218"/>
-      <c r="E56" s="216"/>
-      <c r="F56" s="216"/>
+      <c r="D56" s="184"/>
+      <c r="E56" s="182"/>
+      <c r="F56" s="182"/>
       <c r="G56" s="165"/>
       <c r="J56" s="143">
         <v>7.3</v>
@@ -7815,9 +7815,9 @@
       <c r="A57" s="144"/>
       <c r="B57" s="144"/>
       <c r="C57" s="165"/>
-      <c r="D57" s="218"/>
-      <c r="E57" s="216"/>
-      <c r="F57" s="216"/>
+      <c r="D57" s="184"/>
+      <c r="E57" s="182"/>
+      <c r="F57" s="182"/>
       <c r="G57" s="165"/>
       <c r="K57" s="169"/>
       <c r="L57" s="169"/>
@@ -7826,9 +7826,9 @@
       <c r="A58" s="144"/>
       <c r="B58" s="144"/>
       <c r="C58" s="165"/>
-      <c r="D58" s="218"/>
-      <c r="E58" s="216"/>
-      <c r="F58" s="216"/>
+      <c r="D58" s="184"/>
+      <c r="E58" s="182"/>
+      <c r="F58" s="182"/>
       <c r="G58" s="165"/>
       <c r="H58" s="150"/>
       <c r="I58" s="167" t="s">
@@ -7842,11 +7842,11 @@
       <c r="A59" s="144"/>
       <c r="B59" s="144"/>
       <c r="C59" s="165"/>
-      <c r="D59" s="218"/>
-      <c r="E59" s="216" t="s">
+      <c r="D59" s="184"/>
+      <c r="E59" s="182" t="s">
         <v>407</v>
       </c>
-      <c r="F59" s="216" t="s">
+      <c r="F59" s="182" t="s">
         <v>393</v>
       </c>
       <c r="G59" s="165"/>
@@ -7860,9 +7860,9 @@
       <c r="A60" s="144"/>
       <c r="B60" s="144"/>
       <c r="C60" s="165"/>
-      <c r="D60" s="218"/>
-      <c r="E60" s="216"/>
-      <c r="F60" s="216"/>
+      <c r="D60" s="184"/>
+      <c r="E60" s="182"/>
+      <c r="F60" s="182"/>
       <c r="G60" s="165"/>
       <c r="J60" s="167"/>
       <c r="K60" s="167" t="s">
@@ -7874,9 +7874,9 @@
       <c r="A61" s="144"/>
       <c r="B61" s="144"/>
       <c r="C61" s="165"/>
-      <c r="D61" s="218"/>
-      <c r="E61" s="216"/>
-      <c r="F61" s="216"/>
+      <c r="D61" s="184"/>
+      <c r="E61" s="182"/>
+      <c r="F61" s="182"/>
       <c r="G61" s="165"/>
       <c r="J61" s="169"/>
       <c r="K61" s="169"/>
@@ -7888,9 +7888,9 @@
       <c r="A62" s="144"/>
       <c r="B62" s="144"/>
       <c r="C62" s="165"/>
-      <c r="D62" s="218"/>
-      <c r="E62" s="216"/>
-      <c r="F62" s="216"/>
+      <c r="D62" s="184"/>
+      <c r="E62" s="182"/>
+      <c r="F62" s="182"/>
       <c r="G62" s="165"/>
       <c r="J62" s="169"/>
       <c r="K62" s="169"/>
@@ -7902,18 +7902,18 @@
       <c r="A63" s="144"/>
       <c r="B63" s="144"/>
       <c r="C63" s="165"/>
-      <c r="D63" s="218"/>
-      <c r="E63" s="216"/>
-      <c r="F63" s="216"/>
+      <c r="D63" s="184"/>
+      <c r="E63" s="182"/>
+      <c r="F63" s="182"/>
       <c r="G63" s="165"/>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="144"/>
       <c r="B64" s="144"/>
       <c r="C64" s="165"/>
-      <c r="D64" s="218"/>
-      <c r="E64" s="216"/>
-      <c r="F64" s="216"/>
+      <c r="D64" s="184"/>
+      <c r="E64" s="182"/>
+      <c r="F64" s="182"/>
       <c r="G64" s="165"/>
       <c r="H64" s="150"/>
       <c r="I64" s="167" t="s">
@@ -7931,13 +7931,13 @@
         <v>395</v>
       </c>
       <c r="C65" s="165"/>
-      <c r="D65" s="218" t="s">
+      <c r="D65" s="184" t="s">
         <v>396</v>
       </c>
-      <c r="E65" s="216" t="s">
+      <c r="E65" s="182" t="s">
         <v>397</v>
       </c>
-      <c r="F65" s="216" t="s">
+      <c r="F65" s="182" t="s">
         <v>398</v>
       </c>
       <c r="G65" s="165" t="s">
@@ -7955,12 +7955,12 @@
         <v>404</v>
       </c>
       <c r="C66" s="165"/>
-      <c r="D66" s="218"/>
-      <c r="E66" s="216"/>
-      <c r="F66" s="216" t="s">
+      <c r="D66" s="184"/>
+      <c r="E66" s="182"/>
+      <c r="F66" s="182" t="s">
         <v>408</v>
       </c>
-      <c r="G66" s="214" t="s">
+      <c r="G66" s="180" t="s">
         <v>413</v>
       </c>
       <c r="J66" s="169"/>
@@ -7970,7 +7970,7 @@
       <c r="M66" s="151"/>
     </row>
     <row r="67" spans="1:13">
-      <c r="C67" s="214"/>
+      <c r="C67" s="180"/>
       <c r="D67" s="160"/>
       <c r="E67" s="162"/>
       <c r="F67" s="162"/>
@@ -7981,7 +7981,7 @@
       <c r="M67" s="151"/>
     </row>
     <row r="68" spans="1:13">
-      <c r="C68" s="214"/>
+      <c r="C68" s="180"/>
       <c r="D68" s="160"/>
       <c r="E68" s="162"/>
       <c r="F68" s="162"/>
@@ -8110,16 +8110,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="28.5" customHeight="1" thickBot="1">
-      <c r="A1" s="211" t="s">
+      <c r="A1" s="217" t="s">
         <v>282</v>
       </c>
-      <c r="B1" s="212"/>
-      <c r="C1" s="212"/>
-      <c r="D1" s="212"/>
-      <c r="E1" s="212"/>
-      <c r="F1" s="212"/>
-      <c r="G1" s="212"/>
-      <c r="H1" s="213"/>
+      <c r="B1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="219"/>
     </row>
     <row r="2" spans="1:8" ht="13.5" thickBot="1">
       <c r="A2" s="128" t="s">

</xml_diff>